<commit_message>
ajout de la flotte Sons of Mars
</commit_message>
<xml_diff>
--- a/Fiche Armées/Adeptus Astartes/Sons of Mars/Organisation Sons Of Mars - 834.M41.xlsx
+++ b/Fiche Armées/Adeptus Astartes/Sons of Mars/Organisation Sons Of Mars - 834.M41.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/429d0bbe9bd122b3/Logiciels et Jeux/Warhammer 40000/Campagne et Parties/Fiche Armées/Adeptus Astartes/Sons of Mars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{8A6A9331-CD28-4276-891C-C242EBAA0677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F5A1EE2D-5CFC-E347-B3E6-9596A3696CF2}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{8A6A9331-CD28-4276-891C-C242EBAA0677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7BC506FF-7C03-410B-B9FA-530184D012B2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5059A03F-A345-47A5-8AEB-EB3F85CA9179}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5059A03F-A345-47A5-8AEB-EB3F85CA9179}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chapitre" sheetId="1" r:id="rId1"/>
+    <sheet name="Flotte" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
   <si>
     <t>Compagnie de Vétéran</t>
   </si>
@@ -245,6 +246,206 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Maître de la Flotte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Capitaine , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Maître des Marches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Capitaine , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Maitre des Rites</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Capitaine , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Maître des Victuailles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Capitaine , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seigneur Exécuteur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Capitaine , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Maître des Reliques</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Capitaine , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Maitre des recrues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>1 Dreadnoughts.</t>
+  </si>
+  <si>
+    <t>2 Escouades d'appuis rapproché.</t>
+  </si>
+  <si>
+    <t>1 Dreadnoughts</t>
+  </si>
+  <si>
+    <t>1 Lieutenants.</t>
+  </si>
+  <si>
+    <t>30 Vétérans</t>
+  </si>
+  <si>
+    <t>1 Dreadnoughts.</t>
+  </si>
+  <si>
+    <r>
+      <t>Capitaine Alatus, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Maître de l'Arsenal</t>
     </r>
     <r>
@@ -259,211 +460,20 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Capitaine , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Maître de la Flotte</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Capitaine , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Maître des Marches</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Capitaine , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Maitre des Rites</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Capitaine , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Maître des Victuailles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Capitaine , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Seigneur Exécuteur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Capitaine , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Maître des Reliques</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Capitaine , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Maitre des recrues</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>1 Dreadnoughts.</t>
-  </si>
-  <si>
-    <t>2 Escouades d'appuis rapproché.</t>
-  </si>
-  <si>
-    <t>1 Dreadnoughts</t>
-  </si>
-  <si>
-    <t>1 Lieutenants.</t>
-  </si>
-  <si>
-    <t>30 Vétérans</t>
-  </si>
-  <si>
-    <t>1 Dreadnoughts.</t>
+    <t>Barge de bataille</t>
+  </si>
+  <si>
+    <t>Croiseur d'attaque</t>
+  </si>
+  <si>
+    <t>Spears Of Mars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +556,14 @@
     <font>
       <b/>
       <sz val="9.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -690,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -770,6 +788,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A958CE-2F2C-4B9B-93BF-18CE2A936A79}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,18 +1285,18 @@
         <v>57</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>7</v>
@@ -1294,7 +1313,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>8</v>
@@ -1311,7 +1330,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>9</v>
@@ -1335,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>10</v>
@@ -1347,10 +1366,10 @@
         <v>24</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>12</v>
@@ -1399,19 +1418,19 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1460,6 +1479,54 @@
         <v>27</v>
       </c>
       <c r="E26" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6C4A72-6B49-491C-8EB8-29B6D7DF07AA}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>